<commit_message>
fix a people event bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/RecordInfo.xlsx
+++ b/ConfigData/Xlsx/RecordInfo.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
-    <sheet name="Tilw" sheetId="2" r:id="rId1"/>
+    <sheet name="record" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1410,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>